<commit_message>
Updated task analysis implementation
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56298040-3C68-4BC1-99D5-1407951D1E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99D0D29-E56C-43EE-B3A4-FD32400EC484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23970" yWindow="1830" windowWidth="26580" windowHeight="15555" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3330" yWindow="2220" windowWidth="26520" windowHeight="15555" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ComprehensionTask" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="48">
   <si>
     <t>A</t>
   </si>
@@ -125,40 +125,52 @@
     <t>F_c</t>
   </si>
   <si>
-    <t>IntelligentOffice</t>
-  </si>
-  <si>
-    <t>CleaningRobot</t>
-  </si>
-  <si>
-    <t>Cognitive</t>
-  </si>
-  <si>
-    <t>Cyclomatic</t>
-  </si>
-  <si>
     <t>TDD</t>
   </si>
   <si>
     <t>NO-TDD</t>
   </si>
   <si>
-    <t>Prod</t>
-  </si>
-  <si>
-    <t>Qlty</t>
-  </si>
-  <si>
-    <t>#Tests</t>
-  </si>
-  <si>
     <t>/</t>
   </si>
   <si>
-    <t>#Asserts</t>
-  </si>
-  <si>
-    <t># Smells</t>
+    <t>PROD</t>
+  </si>
+  <si>
+    <t>QLTY</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>ASSERTS</t>
+  </si>
+  <si>
+    <t>SMELLS</t>
+  </si>
+  <si>
+    <t>CYC</t>
+  </si>
+  <si>
+    <t>COG</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>IO</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>46(!)</t>
+  </si>
+  <si>
+    <t>39(!)</t>
   </si>
 </sst>
 </file>
@@ -1498,7 +1510,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1523,25 +1535,25 @@
         <v>5</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="K1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="L1" s="4" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1549,13 +1561,13 @@
         <v>10</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>7</v>
@@ -1567,51 +1579,67 @@
       <c r="H2" s="6">
         <v>10</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="I2" s="6">
+        <v>10</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0</v>
+      </c>
+      <c r="K2" s="6">
+        <v>25</v>
+      </c>
+      <c r="L2" s="6">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="6">
-        <v>13</v>
+        <v>73</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="6">
         <v>10</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
+      <c r="I3" s="6">
+        <v>10</v>
+      </c>
+      <c r="J3" s="6">
+        <v>1</v>
+      </c>
+      <c r="K3" s="6">
+        <v>24</v>
+      </c>
+      <c r="L3" s="6">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>7</v>
@@ -1623,23 +1651,31 @@
       <c r="H4" s="6">
         <v>10</v>
       </c>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
+      <c r="I4" s="6">
+        <v>10</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6">
+        <v>25</v>
+      </c>
+      <c r="L4" s="6">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>8</v>
@@ -1651,23 +1687,31 @@
       <c r="H5" s="6">
         <v>9</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
+      <c r="I5" s="6">
+        <v>9</v>
+      </c>
+      <c r="J5" s="6">
+        <v>1</v>
+      </c>
+      <c r="K5" s="6">
+        <v>18</v>
+      </c>
+      <c r="L5" s="6">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>7</v>
@@ -1679,51 +1723,67 @@
       <c r="H6" s="6">
         <v>8</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
+      <c r="I6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="6">
+        <v>28</v>
+      </c>
+      <c r="L6" s="6">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="6">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6">
         <v>5</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
+      <c r="I7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" s="6">
+        <v>1</v>
+      </c>
+      <c r="K7" s="6">
+        <v>36</v>
+      </c>
+      <c r="L7" s="6">
+        <v>49</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>7</v>
@@ -1735,243 +1795,307 @@
       <c r="H8" s="6">
         <v>10</v>
       </c>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
+      <c r="I8" s="6">
+        <v>10</v>
+      </c>
+      <c r="J8" s="6">
+        <v>1</v>
+      </c>
+      <c r="K8" s="6">
+        <v>21</v>
+      </c>
+      <c r="L8" s="6">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="6">
-        <v>13</v>
+        <v>52</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6">
         <v>12</v>
       </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
+      <c r="I9" s="6">
+        <v>12</v>
+      </c>
+      <c r="J9" s="6">
+        <v>0</v>
+      </c>
+      <c r="K9" s="6">
+        <v>16</v>
+      </c>
+      <c r="L9" s="6">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F10" s="6">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6">
-        <v>3</v>
-      </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="6">
+        <v>0</v>
+      </c>
+      <c r="J10" s="6">
+        <v>0</v>
+      </c>
+      <c r="K10" s="6">
+        <v>16</v>
+      </c>
+      <c r="L10" s="6">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F11" s="6">
-        <v>80</v>
+        <v>17</v>
       </c>
       <c r="G11" s="6"/>
       <c r="H11" s="6">
-        <v>0</v>
-      </c>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="I11" s="6">
+        <v>3</v>
+      </c>
+      <c r="J11" s="6">
+        <v>1</v>
+      </c>
+      <c r="K11" s="6">
+        <v>10</v>
+      </c>
+      <c r="L11" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" s="6">
-        <v>8</v>
+        <v>76</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6">
-        <v>0</v>
-      </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="I12" s="6">
+        <v>7</v>
+      </c>
+      <c r="J12" s="6">
+        <v>1</v>
+      </c>
+      <c r="K12" s="6">
+        <v>16</v>
+      </c>
+      <c r="L12" s="6">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F13" s="6">
-        <v>76</v>
+        <v>8</v>
       </c>
       <c r="G13" s="6"/>
       <c r="H13" s="6">
-        <v>7</v>
-      </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="6">
+        <v>0</v>
+      </c>
+      <c r="J13" s="6">
+        <v>0</v>
+      </c>
+      <c r="K13" s="6">
+        <v>9</v>
+      </c>
+      <c r="L13" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" s="6">
-        <v>21</v>
+        <v>84</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6">
-        <v>13</v>
-      </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="I14" s="6">
+        <v>12</v>
+      </c>
+      <c r="J14" s="6">
+        <v>0</v>
+      </c>
+      <c r="K14" s="6">
+        <v>16</v>
+      </c>
+      <c r="L14" s="6">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F15" s="6">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6">
-        <v>12</v>
-      </c>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
+        <v>13</v>
+      </c>
+      <c r="I15" s="6">
+        <v>13</v>
+      </c>
+      <c r="J15" s="6">
+        <v>2</v>
+      </c>
+      <c r="K15" s="6">
+        <v>19</v>
+      </c>
+      <c r="L15" s="6">
+        <v>40</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0</v>
+      </c>
+      <c r="I16" s="6">
+        <v>0</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -1979,37 +2103,37 @@
         <v>17</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H17" s="6">
-        <v>0</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>41</v>
+        <v>8</v>
+      </c>
+      <c r="I17" s="6">
+        <v>8</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2017,37 +2141,35 @@
         <v>18</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>41</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F18" s="6">
+        <v>56</v>
+      </c>
+      <c r="G18" s="6"/>
       <c r="H18" s="6">
         <v>0</v>
       </c>
-      <c r="I18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>41</v>
+      <c r="I18" s="6">
+        <v>0</v>
+      </c>
+      <c r="J18" s="6">
+        <v>0</v>
+      </c>
+      <c r="K18" s="6">
+        <v>12</v>
+      </c>
+      <c r="L18" s="6">
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2055,37 +2177,35 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>41</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F19" s="6">
+        <v>47</v>
+      </c>
+      <c r="G19" s="6"/>
       <c r="H19" s="6">
-        <v>0</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>41</v>
+        <v>3</v>
+      </c>
+      <c r="I19" s="6">
+        <v>3</v>
+      </c>
+      <c r="J19" s="6">
+        <v>0</v>
+      </c>
+      <c r="K19" s="6">
+        <v>12</v>
+      </c>
+      <c r="L19" s="6">
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>